<commit_message>
Added parameters, added testing for inference
-Hibrid retrieval parameters adjusted for better accuracy -> semantic_weight: float = 0.70, keyword_weight: float = 0.30,
+Added parameter file inference_config.py for testing and streamlit dashboard (like a header in C)
+Added test_inference.py and inference_logger.py for the inference test

------------manual tests---------
-Verified tester (test the tester) workes just as the dashboard inference.
</commit_message>
<xml_diff>
--- a/data/test/Example_Q_and_A_for_RAG_LLM.xlsx
+++ b/data/test/Example_Q_and_A_for_RAG_LLM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T440\Documents\GitHub\ThesisWork\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\00_SW\01_RAG\data\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E56CD98-0EB9-4BF3-B559-9E137BC87A69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA5237B2-B70E-4B68-9EEF-C47DA6D649CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="30960" windowHeight="12120" xr2:uid="{2AFBA614-42DE-4065-86FD-C0FD95C7E89C}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2AFBA614-42DE-4065-86FD-C0FD95C7E89C}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Question</t>
   </si>
@@ -127,6 +127,20 @@
   </si>
   <si>
     <t>What does LDIF stand?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    system_message = """You are a helpful AI assistant specialized in hybrid Retrieval-Augmented Generation (RAG) tasks. Your role is to answer the user's question using both retrieved context from the knowledge base and reasoning based on prior conversation history.
+Always:
+- Analyze the retrieved context carefully before forming an answer.
+- Separate your reasoning process and show it inside &lt;think&gt;&lt;/think&gt; tags. This section should logically outline how you arrive at your conclusion but should never include guesses unrelated to the provided data.
+- Outside the tags, write your final answer clearly, accurately, and concisely in English.
+- If information is missing or unclear, state that explicitly instead of assuming or fabricating details.
+- Ensure all responses are entirely in English, regardless of the query language.
+Example structure:
+&lt;think&gt;
+Step-by-step reasoning and evidence analysis...
+&lt;/think&gt;
+Final, concise answer in English."""</t>
   </si>
 </sst>
 </file>
@@ -511,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6AAC072-CE48-4BBD-A053-AC332D594274}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -619,8 +633,14 @@
         <v>22</v>
       </c>
     </row>
+    <row r="16" spans="1:2" ht="273.60000000000002" x14ac:dyDescent="0.3">
+      <c r="B16" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"Arial"&amp;8&amp;K000000 INTERNAL&amp;1#_x000D_</oddHeader>
   </headerFooter>

</xml_diff>